<commit_message>
ER Diagram Update + Design Document
</commit_message>
<xml_diff>
--- a/usability-report/Report/SUS Survey Data.xlsx
+++ b/usability-report/Report/SUS Survey Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Università\Master - X su 110L\1_Anno\2_Semestre\Hypermedia Application\Repo\Hypermedia-heuristics-evaluation\usability-report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACF9399-E32F-45DE-B858-ADEE31B70C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BEDB13-A039-409D-AF2D-A9F52FDC18AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FBC53F6C-9B8F-4388-A703-0EB7CC628BF7}"/>
   </bookViews>
@@ -356,19 +356,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -417,15 +416,14 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -12467,7 +12465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F4CBEBA-6305-4C2B-A1BF-E6CBEFBE46F9}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
       <selection activeCell="H72" sqref="H72"/>
@@ -12475,102 +12473,100 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.21875" defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.21875" style="4"/>
-    <col min="13" max="13" width="29.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="26.21875" style="4"/>
+    <col min="1" max="1" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="21" t="s">
         <v>28</v>
       </c>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <f>B3-1</f>
         <v>0</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <f>5-C3</f>
         <v>1</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <f>D3-1</f>
         <v>1</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <f>5-E3</f>
         <v>2</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <f>F3-1</f>
         <v>1</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <f>5-G3</f>
         <v>1</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <f>H3-1</f>
         <v>3</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="13">
         <f>5-I3</f>
         <v>2</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="13">
         <f>J3-1</f>
         <v>2</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="14">
         <f>5-K3</f>
         <v>2</v>
       </c>
@@ -12581,83 +12577,83 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>4</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>2</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>3</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>2</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>4</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>4</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="10">
         <v>3</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <v>3</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="17">
         <v>3</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <f>B5-1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <f>5-C5</f>
         <v>2</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <f>D5-1</f>
         <v>2</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <f>5-E5</f>
         <v>4</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <f>F5-1</f>
         <v>1</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <f>5-G5</f>
         <v>1</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <f>H5-1</f>
         <v>3</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <f>5-I5</f>
         <v>1</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <f>J5-1</f>
         <v>3</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="14">
         <f>5-K5</f>
         <v>4</v>
       </c>
@@ -12668,83 +12664,83 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>3</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>3</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>3</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>1</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>2</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>4</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>4</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>4</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>4</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>1</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <f>B7-1</f>
         <v>0</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <f>5-C7</f>
         <v>3</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <f>D7-1</f>
         <v>2</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <f>5-E7</f>
         <v>3</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <f>F7-1</f>
         <v>1</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <f>5-G7</f>
         <v>1</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <f>H7-1</f>
         <v>3</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <f>5-I7</f>
         <v>2</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <f>J7-1</f>
         <v>3</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="14">
         <f>5-K7</f>
         <v>3</v>
       </c>
@@ -12755,83 +12751,83 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>3</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>2</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>2</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>4</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>4</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>3</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>4</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="18">
         <v>2</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <f>B9-1</f>
         <v>2</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <f>5-C9</f>
         <v>3</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <f>D9-1</f>
         <v>3</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <f>5-E9</f>
         <v>4</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <f>F9-1</f>
         <v>2</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <f>5-G9</f>
         <v>1</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <f>H9-1</f>
         <v>2</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <f>5-I9</f>
         <v>3</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <f>J9-1</f>
         <v>3</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="14">
         <f>5-K9</f>
         <v>4</v>
       </c>
@@ -12842,83 +12838,83 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>3</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>2</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>4</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>1</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <v>3</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>4</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>3</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <v>2</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <v>4</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="11">
         <v>1</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <f>B11-1</f>
         <v>2</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <f>5-C11</f>
         <v>3</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <f>D11-1</f>
         <v>3</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <f>5-E11</f>
         <v>3</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <f>F11-1</f>
         <v>3</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <f>5-G11</f>
         <v>3</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <f>H11-1</f>
         <v>3</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <f>5-I11</f>
         <v>3</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <f>J11-1</f>
         <v>3</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="14">
         <f>5-K11</f>
         <v>3</v>
       </c>
@@ -12929,83 +12925,83 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>3</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>2</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>4</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>2</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>4</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>2</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>4</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <v>2</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>4</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="18">
         <v>2</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <f>B13-1</f>
         <v>1</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <f>5-C13</f>
         <v>1</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <f>D13-1</f>
         <v>1</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <f>5-E13</f>
         <v>4</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <f>F13-1</f>
         <v>1</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <f>5-G13</f>
         <v>0</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <f>H13-1</f>
         <v>1</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="13">
         <f>5-I13</f>
         <v>0</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <f>J13-1</f>
         <v>2</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="14">
         <f>5-K13</f>
         <v>1</v>
       </c>
@@ -13016,83 +13012,83 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>2</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>4</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>2</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>1</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>2</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="19">
         <v>5</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="9">
         <v>2</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>5</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="10">
         <v>3</v>
       </c>
-      <c r="K13" s="21">
+      <c r="K13" s="20">
         <v>4</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <f>B15-1</f>
         <v>1</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <f>5-C15</f>
         <v>0</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <f>D15-1</f>
         <v>0</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <f>5-E15</f>
         <v>3</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="13">
         <f>F15-1</f>
         <v>1</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <f>5-G15</f>
         <v>2</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="13">
         <f>H15-1</f>
         <v>1</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <f>5-I15</f>
         <v>1</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <f>J15-1</f>
         <v>1</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="14">
         <f>5-K15</f>
         <v>3</v>
       </c>
@@ -13103,83 +13099,83 @@
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>2</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>5</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>1</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>2</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>2</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="10">
         <v>3</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="9">
         <v>2</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="8">
         <v>4</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="9">
         <v>2</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="18">
         <v>2</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <f>B17-1</f>
         <v>1</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="13">
         <f>5-C17</f>
         <v>2</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <f>D17-1</f>
         <v>2</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <f>5-E17</f>
         <v>4</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <f>F17-1</f>
         <v>1</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <f>5-G17</f>
         <v>1</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <f>H17-1</f>
         <v>4</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <f>5-I17</f>
         <v>1</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <f>J17-1</f>
         <v>2</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="14">
         <f>5-K17</f>
         <v>4</v>
       </c>
@@ -13190,83 +13186,83 @@
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>2</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>3</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>3</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="16">
         <v>1</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>2</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <v>4</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="19">
         <v>5</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="8">
         <v>4</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="10">
         <v>3</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="11">
         <v>1</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <f>B19-1</f>
         <v>1</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <f>5-C19</f>
         <v>1</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <f>D19-1</f>
         <v>3</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <f>5-E19</f>
         <v>3</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="13">
         <f>F19-1</f>
         <v>1</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <f>5-G19</f>
         <v>2</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="13">
         <f>H19-1</f>
         <v>3</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="13">
         <f>5-I19</f>
         <v>2</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <f>J19-1</f>
         <v>3</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="14">
         <f>5-K19</f>
         <v>4</v>
       </c>
@@ -13277,131 +13273,122 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>2</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>4</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>4</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>2</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <v>2</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="10">
         <v>3</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>4</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="10">
         <v>3</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <v>4</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="11">
         <v>1</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="25">
+      <c r="B20" s="24">
         <f>SUM(B3,B5,B7,B9,B11,B13,B15,B17,B19) / 9</f>
         <v>2.1111111111111112</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20">
         <f>SUM(C3,C5,C7,C9,C11,C13,C15,C17,C19) / 9</f>
         <v>3.2222222222222223</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20">
         <f t="shared" ref="D20:K20" si="0">SUM(D3,D5,D7,D9,D11,D13,D15,D17,D19) / 9</f>
         <v>2.8888888888888888</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="23">
         <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20">
         <f t="shared" si="0"/>
         <v>2.3333333333333335</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="23">
         <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="24">
         <f t="shared" si="0"/>
         <v>3.5555555555555554</v>
       </c>
-      <c r="I20" s="26">
+      <c r="I20">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="J20" s="26">
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>3.4444444444444446</v>
       </c>
-      <c r="K20" s="26">
+      <c r="K20">
         <f t="shared" si="0"/>
         <v>1.8888888888888888</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20">
         <f xml:space="preserve"> SUM(L2,L4,L6,L8,L10,L12,L14,L16,L18) / 9</f>
         <v>51.388888888888886</v>
       </c>
-      <c r="M20" s="23" t="s">
+      <c r="M20" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H21" t="s">
         <v>30</v>
       </c>
-      <c r="I21" s="26" t="s">
+      <c r="I21" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="26" t="s">
+      <c r="J21" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="K21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>